<commit_message>
Added code for hash
</commit_message>
<xml_diff>
--- a/Sharkspray/JSON_TC/Features/Sharkspray_Testcases.xlsx
+++ b/Sharkspray/JSON_TC/Features/Sharkspray_Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\ss-git\sharkspray_script\Sharkspray\JSON_TC\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D617D9-A121-4566-8779-C009706F26C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A6266E-029C-40C6-8809-2415CC5D0C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2B78A716-6A39-4C80-A30F-171CE75D3BE3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Sno.</t>
   </si>
@@ -96,7 +96,25 @@
     <t>PSA - Adhesive Transfer Tape (ATT)</t>
   </si>
   <si>
-    <t>PSA - Adhesive Transfer Tape (ATT</t>
+    <t>oca2_p3</t>
+  </si>
+  <si>
+    <t>oca2_dma.xml</t>
+  </si>
+  <si>
+    <t>oca2_compression.xml</t>
+  </si>
+  <si>
+    <t>oca2_tension.xlsx</t>
+  </si>
+  <si>
+    <t>Phase 3 (DMA + Compression + Tension)</t>
+  </si>
+  <si>
+    <t>oca2_p3_ModelFiles.zip</t>
+  </si>
+  <si>
+    <t>Tension</t>
   </si>
 </sst>
 </file>
@@ -448,20 +466,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF14122-9760-46AA-9668-A2F1AAE2BA4F}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.77734375" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="7" max="7" width="29.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="34.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.77734375" customWidth="1"/>
     <col min="10" max="10" width="15.21875" customWidth="1"/>
     <col min="11" max="11" width="22.21875" customWidth="1"/>
@@ -545,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
@@ -555,6 +573,41 @@
       </c>
       <c r="J3" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>